<commit_message>
- fixed bug with empty calls in 'Data_prepared' - minor chnages with printing content
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/Products/jet_fuel/Model_Data_Base_jet_fuel.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/Products/jet_fuel/Model_Data_Base_jet_fuel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/Products/jet_fuel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kar.eco\github_repos\Nord_H2ub\Spine_Projects\01_input_data\01_input_raw\Products\jet_fuel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{384EF942-1BB3-4AF5-A4C8-1EAD5F73D2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CBDAA88-D274-4E38-B411-90287AD514EF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02DA6B8-E6CE-43B1-ADE7-2080F52F0861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -1234,17 +1234,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1300,7 +1316,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -1313,7 +1329,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -1326,7 +1342,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -1339,7 +1355,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -1361,7 +1377,7 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -1374,7 +1390,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -1387,7 +1403,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>70</v>
       </c>
@@ -1400,7 +1416,7 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>89</v>
       </c>
@@ -1416,7 +1432,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>73</v>
       </c>
@@ -1435,7 +1451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>117</v>
       </c>
@@ -1450,7 +1466,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>100</v>
       </c>
@@ -1463,7 +1479,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>101</v>
       </c>
@@ -1476,7 +1492,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>116</v>
       </c>
@@ -1505,17 +1521,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8478C130-C296-4571-ABF4-62E91E9E2767}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1568,7 +1593,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
@@ -1593,7 +1618,7 @@
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>96</v>
       </c>
@@ -1618,7 +1643,7 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -1643,7 +1668,7 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>64</v>
       </c>
@@ -1678,7 +1703,7 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>67</v>
       </c>
@@ -1711,7 +1736,7 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -1748,7 +1773,7 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -1789,7 +1814,7 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>89</v>
       </c>
@@ -1822,7 +1847,7 @@
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>100</v>
       </c>
@@ -1839,7 +1864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>101</v>
       </c>
@@ -1868,7 +1893,7 @@
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -1915,7 +1940,7 @@
       </c>
       <c r="Q12" s="9"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>117</v>
       </c>
@@ -1944,7 +1969,7 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>116</v>
       </c>
@@ -1986,37 +2011,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA5" sqref="AA5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="36.54296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2099,7 +2124,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -2158,7 +2183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -2214,7 +2239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>90</v>
       </c>
@@ -2240,7 +2265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -2293,20 +2318,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -2341,7 +2366,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -2367,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>85</v>
       </c>
@@ -2419,102 +2444,102 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>95</v>
       </c>

</xml_diff>